<commit_message>
code clean up for grade title
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/externalframework/exf_ingestion_all_fields/ExF_Ingestion_all_fields.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/externalframework/exf_ingestion_all_fields/ExF_Ingestion_all_fields.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
   <si>
     <t>Unique id</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Ability to tap into the interdisciplinary nature of science</t>
-  </si>
-  <si>
-    <t>AAAS</t>
   </si>
   <si>
     <t>CCE A1</t>
@@ -693,7 +690,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A8:A9"/>
+      <selection activeCell="D3" sqref="D3:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -711,7 +708,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -745,19 +742,17 @@
     </row>
     <row r="3" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>8</v>
@@ -765,16 +760,14 @@
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="3">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -790,11 +783,9 @@
       <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>11</v>
@@ -805,16 +796,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="3">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>12</v>
@@ -830,11 +819,9 @@
       <c r="C7" s="3">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
@@ -845,16 +832,14 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>14</v>
@@ -870,11 +855,9 @@
       <c r="C9" s="3">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>15</v>
@@ -890,11 +873,9 @@
       <c r="C10" s="3">
         <v>12</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>16</v>
@@ -910,11 +891,9 @@
       <c r="C11" s="3">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
@@ -930,11 +909,9 @@
       <c r="C12" s="3">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>18</v>
@@ -950,11 +927,9 @@
       <c r="C13" s="3">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>19</v>
@@ -967,11 +942,9 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>20</v>
@@ -984,11 +957,9 @@
       <c r="C15" s="3">
         <v>12</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>21</v>
@@ -1001,11 +972,9 @@
       <c r="C16" s="3">
         <v>12</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>11</v>
@@ -1018,11 +987,9 @@
       <c r="C17" s="3">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>22</v>
@@ -1035,11 +1002,9 @@
       <c r="C18" s="3">
         <v>12</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>13</v>
@@ -1052,11 +1017,9 @@
       <c r="C19" s="3">
         <v>12</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>23</v>
@@ -1069,11 +1032,9 @@
       <c r="C20" s="3">
         <v>12</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
@@ -1086,11 +1047,9 @@
       <c r="C21" s="3">
         <v>12</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>24</v>
@@ -1103,11 +1062,9 @@
       <c r="C22" s="3">
         <v>12</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>25</v>
@@ -1120,11 +1077,9 @@
       <c r="C23" s="3">
         <v>12</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>26</v>
@@ -1137,11 +1092,9 @@
       <c r="C24" s="3">
         <v>12</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>27</v>
@@ -1154,11 +1107,9 @@
       <c r="C25" s="3">
         <v>12</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>28</v>
@@ -1171,11 +1122,9 @@
       <c r="C26" s="3">
         <v>12</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>11</v>
@@ -1188,11 +1137,9 @@
       <c r="C27" s="3">
         <v>12</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>29</v>
@@ -1205,11 +1152,9 @@
       <c r="C28" s="3">
         <v>12</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>13</v>
@@ -1222,11 +1167,9 @@
       <c r="C29" s="3">
         <v>12</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>30</v>
@@ -1239,11 +1182,9 @@
       <c r="C30" s="3">
         <v>12</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>15</v>
@@ -1256,11 +1197,9 @@
       <c r="C31" s="3">
         <v>12</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>31</v>
@@ -1273,11 +1212,9 @@
       <c r="C32" s="3">
         <v>12</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>32</v>
@@ -1290,14 +1227,12 @@
       <c r="C33" s="3">
         <v>12</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
@@ -1307,11 +1242,9 @@
       <c r="C34" s="3">
         <v>12</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>11</v>
@@ -1324,11 +1257,9 @@
       <c r="C35" s="3">
         <v>12</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>10</v>
@@ -1341,11 +1272,9 @@
       <c r="C36" s="3">
         <v>12</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>12</v>
@@ -1358,11 +1287,9 @@
       <c r="C37" s="3">
         <v>12</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>21</v>
@@ -1375,11 +1302,9 @@
       <c r="C38" s="3">
         <v>12</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>22</v>
@@ -1392,11 +1317,9 @@
       <c r="C39" s="3">
         <v>12</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>28</v>
@@ -1409,11 +1332,9 @@
       <c r="C40" s="3">
         <v>12</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>29</v>
@@ -1426,11 +1347,9 @@
       <c r="C41" s="3">
         <v>12</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>33</v>
@@ -1443,11 +1362,9 @@
       <c r="C42" s="3">
         <v>12</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>13</v>
@@ -1460,11 +1377,9 @@
       <c r="C43" s="3">
         <v>12</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>10</v>
@@ -1477,11 +1392,9 @@
       <c r="C44" s="3">
         <v>12</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>14</v>
@@ -1494,11 +1407,9 @@
       <c r="C45" s="3">
         <v>12</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>21</v>
@@ -1511,11 +1422,9 @@
       <c r="C46" s="3">
         <v>12</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>23</v>
@@ -1528,11 +1437,9 @@
       <c r="C47" s="3">
         <v>12</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>28</v>
@@ -1545,11 +1452,9 @@
       <c r="C48" s="3">
         <v>12</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>30</v>
@@ -1562,11 +1467,9 @@
       <c r="C49" s="3">
         <v>12</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>33</v>
@@ -1579,11 +1482,9 @@
       <c r="C50" s="3">
         <v>12</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>15</v>
@@ -1596,11 +1497,9 @@
       <c r="C51" s="3">
         <v>12</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>10</v>
@@ -1613,11 +1512,9 @@
       <c r="C52" s="3">
         <v>12</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>16</v>
@@ -1630,11 +1527,9 @@
       <c r="C53" s="3">
         <v>12</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>17</v>
@@ -1647,11 +1542,9 @@
       <c r="C54" s="3">
         <v>12</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>18</v>
@@ -1664,11 +1557,9 @@
       <c r="C55" s="3">
         <v>12</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>19</v>
@@ -1681,11 +1572,9 @@
       <c r="C56" s="3">
         <v>12</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>20</v>
@@ -1698,11 +1587,9 @@
       <c r="C57" s="3">
         <v>12</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>21</v>
@@ -1715,11 +1602,9 @@
       <c r="C58" s="3">
         <v>12</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>24</v>
@@ -1732,11 +1617,9 @@
       <c r="C59" s="3">
         <v>12</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>25</v>
@@ -1749,11 +1632,9 @@
       <c r="C60" s="3">
         <v>12</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>26</v>
@@ -1767,11 +1648,9 @@
       <c r="C61" s="3">
         <v>12</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>27</v>
@@ -1784,11 +1663,9 @@
       <c r="C62" s="3">
         <v>12</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>28</v>
@@ -1801,11 +1678,9 @@
       <c r="C63" s="3">
         <v>12</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>31</v>
@@ -1818,11 +1693,9 @@
       <c r="C64" s="3">
         <v>12</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
exf code clean up
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/externalframework/exf_ingestion_all_fields/ExF_Ingestion_all_fields.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/externalframework/exf_ingestion_all_fields/ExF_Ingestion_all_fields.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lomt_automation\src\main\java\lomt\pearson\fileupload\externalframework\exf_ingestion_all_fields\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ram.sin\Desktop\EXF-changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
   <si>
     <t>Unique id</t>
   </si>
@@ -321,7 +321,16 @@
     <t>PK</t>
   </si>
   <si>
-    <t>External Frameworks-Test_Automation-23feb</t>
+    <t>Abacus|Maclaurin's series|T-test|UK currency</t>
+  </si>
+  <si>
+    <t>UK currency</t>
+  </si>
+  <si>
+    <t>Maclaurin's series|UK currency</t>
+  </si>
+  <si>
+    <t>External Frameworks-Test_Automation-11March-18</t>
   </si>
 </sst>
 </file>
@@ -689,7 +698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -699,14 +710,14 @@
     <col min="4" max="4" width="30.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="21.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="91.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -752,8 +763,8 @@
       <c r="F3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>8</v>
+      <c r="I3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -771,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -789,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -962,6 +973,9 @@
       <c r="F15" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="I15" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
@@ -978,7 +992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>12</v>
       </c>
@@ -993,7 +1007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>12</v>
       </c>
@@ -1008,7 +1022,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>12</v>
       </c>
@@ -1023,7 +1037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>12</v>
       </c>
@@ -1038,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>12</v>
       </c>
@@ -1053,7 +1067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>12</v>
       </c>
@@ -1068,7 +1082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>12</v>
       </c>
@@ -1083,7 +1097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>12</v>
       </c>
@@ -1097,8 +1111,11 @@
       <c r="H24" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>12</v>
       </c>
@@ -1113,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>12</v>
       </c>
@@ -1128,7 +1145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>12</v>
       </c>
@@ -1143,7 +1160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>12</v>
       </c>
@@ -1158,7 +1175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -1173,7 +1190,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>12</v>
       </c>
@@ -1188,7 +1205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>12</v>
       </c>
@@ -1203,7 +1220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>12</v>
       </c>
@@ -1293,7 +1310,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B38" s="1">
         <v>12</v>
       </c>
@@ -1443,7 +1460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B48" s="1">
         <v>12</v>
       </c>
@@ -1458,7 +1475,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
         <v>12</v>
       </c>
@@ -1473,7 +1490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <v>12</v>
       </c>
@@ -1487,8 +1504,11 @@
       <c r="F50" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
         <v>12</v>
       </c>
@@ -1502,8 +1522,11 @@
       <c r="G51" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
         <v>12</v>
       </c>
@@ -1517,8 +1540,11 @@
       <c r="H52" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
         <v>12</v>
       </c>
@@ -1533,7 +1559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <v>12</v>
       </c>
@@ -1548,7 +1574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <v>12</v>
       </c>
@@ -1563,7 +1589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B56" s="1">
         <v>12</v>
       </c>
@@ -1578,7 +1604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B57" s="1">
         <v>12</v>
       </c>
@@ -1593,7 +1619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="1">
         <v>12</v>
       </c>
@@ -1608,7 +1634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <v>12</v>
       </c>
@@ -1623,7 +1649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <v>12</v>
       </c>
@@ -1638,7 +1664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="1">
         <v>12</v>
@@ -1654,7 +1680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <v>12</v>
       </c>
@@ -1668,8 +1694,11 @@
       <c r="G62" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
         <v>12</v>
       </c>
@@ -1683,8 +1712,11 @@
       <c r="H63" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
         <v>12</v>
       </c>
@@ -1697,6 +1729,9 @@
       </c>
       <c r="H64" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="I64" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>